<commit_message>
- Følgende mapper er oprettet: System1(ACME), SHA1(HASH) og Common(email). - Der er oprettet følgende workflows i mapperne: Login, Luk applikationer, naviger til workitem
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\FørsteProjekt\Calculate_Client_Security_Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C0B97F-C5C7-48D9-8B10-E7967207F2EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,19 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>Brugernavn og PW til ACME</t>
+  </si>
+  <si>
+    <t>ACME_URL</t>
+  </si>
+  <si>
+    <t>ACME_Credential</t>
+  </si>
+  <si>
+    <t>Hash_URL</t>
+  </si>
+  <si>
+    <t>Calculate_client_security_hash</t>
   </si>
 </sst>
 </file>
@@ -177,6 +189,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -239,7 +252,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -538,15 +551,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -587,24 +600,24 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -616,7 +629,17 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1619,16 +1642,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,18 +1688,18 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1813,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2782,14 +2805,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2828,8 +2853,22 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>